<commit_message>
Bonn Budget New Code Lists
Added/updated pipeline + turtle file for 3 code lists: costCenter,
internalOrder and pspElement.

Added those in the dataset as well.
</commit_message>
<xml_diff>
--- a/Bonn/raw/PSP-Elemente2016.xlsx
+++ b/Bonn/raw/PSP-Elemente2016.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="676">
   <si>
     <t>Politische Gremien</t>
   </si>
@@ -2041,19 +2041,28 @@
   </si>
   <si>
     <t>Profit Center</t>
+  </si>
+  <si>
+    <t>Amt</t>
+  </si>
+  <si>
+    <t>Produkt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2066,8 +2075,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2090,15 +2105,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2405,10 +2451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C263"/>
+  <dimension ref="A1:E263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2416,9 +2462,10 @@
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>671</v>
       </c>
@@ -2428,8 +2475,14 @@
       <c r="C1" s="1" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="4" t="s">
+        <v>674</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2439,8 +2492,14 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2450,8 +2509,14 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="2">
+        <v>200</v>
+      </c>
+      <c r="E3" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2461,8 +2526,14 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="2">
+        <v>200</v>
+      </c>
+      <c r="E4" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2472,8 +2543,14 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="2">
+        <v>200</v>
+      </c>
+      <c r="E5" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2483,8 +2560,14 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="2">
+        <v>200</v>
+      </c>
+      <c r="E6" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2494,8 +2577,14 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="2">
+        <v>200</v>
+      </c>
+      <c r="E7" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2505,8 +2594,14 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E8" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2516,8 +2611,14 @@
       <c r="C9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="2">
+        <v>400</v>
+      </c>
+      <c r="E9" s="2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -2527,8 +2628,14 @@
       <c r="C10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" s="2">
+        <v>1400</v>
+      </c>
+      <c r="E10" s="2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -2538,8 +2645,14 @@
       <c r="C11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E11" s="2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2549,8 +2662,14 @@
       <c r="C12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2560,8 +2679,14 @@
       <c r="C13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E13" s="2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2571,8 +2696,14 @@
       <c r="C14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E14" s="2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2582,8 +2713,14 @@
       <c r="C15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E15" s="2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2593,8 +2730,14 @@
       <c r="C16" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E16" s="2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2604,8 +2747,14 @@
       <c r="C17" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="2">
+        <v>1300</v>
+      </c>
+      <c r="E17" s="2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -2615,8 +2764,14 @@
       <c r="C18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="2">
+        <v>1300</v>
+      </c>
+      <c r="E18" s="2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -2626,8 +2781,14 @@
       <c r="C19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="2">
+        <v>1300</v>
+      </c>
+      <c r="E19" s="2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -2637,8 +2798,14 @@
       <c r="C20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="2">
+        <v>1300</v>
+      </c>
+      <c r="E20" s="2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -2648,8 +2815,14 @@
       <c r="C21" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="2">
+        <v>1100</v>
+      </c>
+      <c r="E21" s="2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -2659,8 +2832,14 @@
       <c r="C22" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="2">
+        <v>1100</v>
+      </c>
+      <c r="E22" s="2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -2670,8 +2849,14 @@
       <c r="C23" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" s="2">
+        <v>1100</v>
+      </c>
+      <c r="E23" s="2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -2681,8 +2866,14 @@
       <c r="C24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" s="2">
+        <v>1100</v>
+      </c>
+      <c r="E24" s="2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2692,8 +2883,14 @@
       <c r="C25" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" s="2">
+        <v>1100</v>
+      </c>
+      <c r="E25" s="2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2703,8 +2900,14 @@
       <c r="C26" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" s="2">
+        <v>1100</v>
+      </c>
+      <c r="E26" s="2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -2714,8 +2917,14 @@
       <c r="C27" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" s="2">
+        <v>200</v>
+      </c>
+      <c r="E27" s="2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -2725,8 +2934,14 @@
       <c r="C28" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E28" s="2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -2736,8 +2951,14 @@
       <c r="C29" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E29" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -2747,8 +2968,14 @@
       <c r="C30" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E30" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -2758,8 +2985,14 @@
       <c r="C31" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E31" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -2769,8 +3002,14 @@
       <c r="C32" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E32" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -2780,8 +3019,14 @@
       <c r="C33" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" s="2">
+        <v>2100</v>
+      </c>
+      <c r="E33" s="2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -2791,8 +3036,14 @@
       <c r="C34" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" s="2">
+        <v>2100</v>
+      </c>
+      <c r="E34" s="2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2802,8 +3053,14 @@
       <c r="C35" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" s="2">
+        <v>2100</v>
+      </c>
+      <c r="E35" s="2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -2813,8 +3070,14 @@
       <c r="C36" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E36" s="2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -2824,8 +3087,14 @@
       <c r="C37" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E37" s="2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -2835,8 +3104,14 @@
       <c r="C38" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" s="2">
+        <v>1020</v>
+      </c>
+      <c r="E38" s="2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -2846,8 +3121,14 @@
       <c r="C39" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E39" s="2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -2857,8 +3138,14 @@
       <c r="C40" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E40" s="2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>99</v>
       </c>
@@ -2868,8 +3155,14 @@
       <c r="C41" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E41" s="2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>101</v>
       </c>
@@ -2879,8 +3172,14 @@
       <c r="C42" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E42" s="2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>103</v>
       </c>
@@ -2890,8 +3189,14 @@
       <c r="C43" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" s="2">
+        <v>2300</v>
+      </c>
+      <c r="E43" s="2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>106</v>
       </c>
@@ -2901,8 +3206,14 @@
       <c r="C44" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" s="2">
+        <v>2300</v>
+      </c>
+      <c r="E44" s="2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>108</v>
       </c>
@@ -2912,8 +3223,14 @@
       <c r="C45" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" s="2">
+        <v>2300</v>
+      </c>
+      <c r="E45" s="2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>110</v>
       </c>
@@ -2923,8 +3240,14 @@
       <c r="C46" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" s="2">
+        <v>2010</v>
+      </c>
+      <c r="E46" s="2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>113</v>
       </c>
@@ -2934,8 +3257,14 @@
       <c r="C47" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" s="2">
+        <v>1066</v>
+      </c>
+      <c r="E47" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>116</v>
       </c>
@@ -2945,8 +3274,14 @@
       <c r="C48" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" s="2">
+        <v>1077</v>
+      </c>
+      <c r="E48" s="2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>119</v>
       </c>
@@ -2956,8 +3291,14 @@
       <c r="C49" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" s="2">
+        <v>1077</v>
+      </c>
+      <c r="E49" s="2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>121</v>
       </c>
@@ -2967,8 +3308,14 @@
       <c r="C50" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" s="2">
+        <v>1088</v>
+      </c>
+      <c r="E50" s="2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>124</v>
       </c>
@@ -2978,8 +3325,14 @@
       <c r="C51" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" s="2">
+        <v>1099</v>
+      </c>
+      <c r="E51" s="2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>127</v>
       </c>
@@ -2989,8 +3342,14 @@
       <c r="C52" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" s="2">
+        <v>1099</v>
+      </c>
+      <c r="E52" s="2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>129</v>
       </c>
@@ -3000,8 +3359,14 @@
       <c r="C53" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E53" s="2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>132</v>
       </c>
@@ -3011,8 +3376,14 @@
       <c r="C54" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E54" s="2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>134</v>
       </c>
@@ -3022,8 +3393,14 @@
       <c r="C55" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E55" s="2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>136</v>
       </c>
@@ -3033,8 +3410,14 @@
       <c r="C56" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E56" s="2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>138</v>
       </c>
@@ -3044,8 +3427,14 @@
       <c r="C57" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E57" s="2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>140</v>
       </c>
@@ -3055,8 +3444,14 @@
       <c r="C58" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E58" s="2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>143</v>
       </c>
@@ -3066,8 +3461,14 @@
       <c r="C59" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E59" s="2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>145</v>
       </c>
@@ -3077,8 +3478,14 @@
       <c r="C60" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E60" s="2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>148</v>
       </c>
@@ -3088,8 +3495,14 @@
       <c r="C61" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E61" s="2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>150</v>
       </c>
@@ -3099,8 +3512,14 @@
       <c r="C62" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E62" s="2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>152</v>
       </c>
@@ -3110,8 +3529,14 @@
       <c r="C63" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E63" s="2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>155</v>
       </c>
@@ -3121,8 +3546,14 @@
       <c r="C64" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E64" s="2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>157</v>
       </c>
@@ -3132,8 +3563,14 @@
       <c r="C65" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E65" s="2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>159</v>
       </c>
@@ -3143,8 +3580,14 @@
       <c r="C66" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E66" s="2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>161</v>
       </c>
@@ -3154,8 +3597,14 @@
       <c r="C67" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E67" s="2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>163</v>
       </c>
@@ -3165,8 +3614,14 @@
       <c r="C68" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E68" s="2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>166</v>
       </c>
@@ -3176,8 +3631,14 @@
       <c r="C69" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E69" s="2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>168</v>
       </c>
@@ -3187,8 +3648,14 @@
       <c r="C70" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E70" s="2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>170</v>
       </c>
@@ -3198,8 +3665,14 @@
       <c r="C71" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E71" s="2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>173</v>
       </c>
@@ -3209,8 +3682,14 @@
       <c r="C72" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E72" s="2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>175</v>
       </c>
@@ -3220,8 +3699,14 @@
       <c r="C73" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E73" s="2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>177</v>
       </c>
@@ -3231,8 +3716,14 @@
       <c r="C74" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E74" s="2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>179</v>
       </c>
@@ -3242,8 +3733,14 @@
       <c r="C75" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75" s="2">
+        <v>3300</v>
+      </c>
+      <c r="E75" s="2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>183</v>
       </c>
@@ -3253,8 +3750,14 @@
       <c r="C76" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76" s="2">
+        <v>5600</v>
+      </c>
+      <c r="E76" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>185</v>
       </c>
@@ -3264,8 +3767,14 @@
       <c r="C77" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77" s="2">
+        <v>6100</v>
+      </c>
+      <c r="E77" s="2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>188</v>
       </c>
@@ -3275,8 +3784,14 @@
       <c r="C78" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78" s="2">
+        <v>3700</v>
+      </c>
+      <c r="E78" s="2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>191</v>
       </c>
@@ -3286,8 +3801,14 @@
       <c r="C79" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79" s="2">
+        <v>3700</v>
+      </c>
+      <c r="E79" s="2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>193</v>
       </c>
@@ -3297,8 +3818,14 @@
       <c r="C80" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80" s="2">
+        <v>3700</v>
+      </c>
+      <c r="E80" s="2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>196</v>
       </c>
@@ -3308,8 +3835,14 @@
       <c r="C81" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81" s="2">
+        <v>3700</v>
+      </c>
+      <c r="E81" s="2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>199</v>
       </c>
@@ -3319,8 +3852,14 @@
       <c r="C82" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82" s="2">
+        <v>3700</v>
+      </c>
+      <c r="E82" s="2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>201</v>
       </c>
@@ -3330,8 +3869,14 @@
       <c r="C83" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83" s="2">
+        <v>3700</v>
+      </c>
+      <c r="E83" s="2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>203</v>
       </c>
@@ -3341,8 +3886,14 @@
       <c r="C84" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E84" s="2">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>206</v>
       </c>
@@ -3352,8 +3903,14 @@
       <c r="C85" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E85" s="2">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>209</v>
       </c>
@@ -3363,8 +3920,14 @@
       <c r="C86" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E86" s="2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>212</v>
       </c>
@@ -3374,8 +3937,14 @@
       <c r="C87" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E87" s="2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>215</v>
       </c>
@@ -3385,8 +3954,14 @@
       <c r="C88" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E88" s="2">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>218</v>
       </c>
@@ -3396,8 +3971,14 @@
       <c r="C89" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E89" s="2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>221</v>
       </c>
@@ -3407,8 +3988,14 @@
       <c r="C90" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E90" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>224</v>
       </c>
@@ -3418,8 +4005,14 @@
       <c r="C91" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D91" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E91" s="2">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>227</v>
       </c>
@@ -3429,8 +4022,14 @@
       <c r="C92" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D92" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E92" s="2">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>230</v>
       </c>
@@ -3440,8 +4039,14 @@
       <c r="C93" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E93" s="2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>233</v>
       </c>
@@ -3451,8 +4056,14 @@
       <c r="C94" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94" s="2">
+        <v>4100</v>
+      </c>
+      <c r="E94" s="2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>236</v>
       </c>
@@ -3462,8 +4073,14 @@
       <c r="C95" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95" s="2">
+        <v>4100</v>
+      </c>
+      <c r="E95" s="2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>239</v>
       </c>
@@ -3473,8 +4090,14 @@
       <c r="C96" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D96" s="2">
+        <v>4100</v>
+      </c>
+      <c r="E96" s="2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>241</v>
       </c>
@@ -3484,8 +4107,14 @@
       <c r="C97" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97" s="2">
+        <v>4100</v>
+      </c>
+      <c r="E97" s="2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>244</v>
       </c>
@@ -3495,8 +4124,14 @@
       <c r="C98" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98" s="2">
+        <v>4100</v>
+      </c>
+      <c r="E98" s="2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>246</v>
       </c>
@@ -3506,8 +4141,14 @@
       <c r="C99" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99" s="2">
+        <v>4180</v>
+      </c>
+      <c r="E99" s="2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>250</v>
       </c>
@@ -3517,8 +4158,14 @@
       <c r="C100" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D100" s="2">
+        <v>4170</v>
+      </c>
+      <c r="E100" s="2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>252</v>
       </c>
@@ -3528,8 +4175,14 @@
       <c r="C101" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D101" s="2">
+        <v>4170</v>
+      </c>
+      <c r="E101" s="2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>254</v>
       </c>
@@ -3539,8 +4192,14 @@
       <c r="C102" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D102" s="2">
+        <v>4170</v>
+      </c>
+      <c r="E102" s="2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>256</v>
       </c>
@@ -3550,8 +4209,14 @@
       <c r="C103" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D103" s="2">
+        <v>4170</v>
+      </c>
+      <c r="E103" s="2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>258</v>
       </c>
@@ -3561,8 +4226,14 @@
       <c r="C104" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D104" s="2">
+        <v>4170</v>
+      </c>
+      <c r="E104" s="2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>260</v>
       </c>
@@ -3572,8 +4243,14 @@
       <c r="C105" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D105" s="2">
+        <v>4170</v>
+      </c>
+      <c r="E105" s="2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>262</v>
       </c>
@@ -3583,8 +4260,14 @@
       <c r="C106" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D106" s="2">
+        <v>4170</v>
+      </c>
+      <c r="E106" s="2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>264</v>
       </c>
@@ -3594,8 +4277,14 @@
       <c r="C107" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D107" s="2">
+        <v>4160</v>
+      </c>
+      <c r="E107" s="2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>267</v>
       </c>
@@ -3605,8 +4294,14 @@
       <c r="C108" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D108" s="2">
+        <v>4140</v>
+      </c>
+      <c r="E108" s="2">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>270</v>
       </c>
@@ -3616,8 +4311,14 @@
       <c r="C109" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D109" s="2">
+        <v>4150</v>
+      </c>
+      <c r="E109" s="2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>273</v>
       </c>
@@ -3627,8 +4328,14 @@
       <c r="C110" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D110" s="2">
+        <v>4150</v>
+      </c>
+      <c r="E110" s="2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>275</v>
       </c>
@@ -3638,8 +4345,14 @@
       <c r="C111" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D111" s="2">
+        <v>4130</v>
+      </c>
+      <c r="E111" s="2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>277</v>
       </c>
@@ -3649,8 +4362,14 @@
       <c r="C112" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D112" s="2">
+        <v>4130</v>
+      </c>
+      <c r="E112" s="2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>279</v>
       </c>
@@ -3660,8 +4379,14 @@
       <c r="C113" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D113" s="2">
+        <v>4120</v>
+      </c>
+      <c r="E113" s="2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>282</v>
       </c>
@@ -3671,8 +4396,14 @@
       <c r="C114" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D114" s="2">
+        <v>4120</v>
+      </c>
+      <c r="E114" s="2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>284</v>
       </c>
@@ -3682,8 +4413,14 @@
       <c r="C115" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D115" s="2">
+        <v>4190</v>
+      </c>
+      <c r="E115" s="2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>287</v>
       </c>
@@ -3693,8 +4430,14 @@
       <c r="C116" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D116" s="2">
+        <v>9040</v>
+      </c>
+      <c r="E116" s="2">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>290</v>
       </c>
@@ -3704,8 +4447,14 @@
       <c r="C117" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D117" s="2">
+        <v>9040</v>
+      </c>
+      <c r="E117" s="2">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>293</v>
       </c>
@@ -3715,8 +4464,14 @@
       <c r="C118" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D118" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E118" s="2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>296</v>
       </c>
@@ -3726,8 +4481,14 @@
       <c r="C119" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D119" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E119" s="2">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>299</v>
       </c>
@@ -3737,8 +4498,14 @@
       <c r="C120" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D120" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E120" s="2">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>301</v>
       </c>
@@ -3748,8 +4515,14 @@
       <c r="C121" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D121" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E121" s="2">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>304</v>
       </c>
@@ -3759,8 +4532,14 @@
       <c r="C122" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D122" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E122" s="2">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>306</v>
       </c>
@@ -3770,8 +4549,14 @@
       <c r="C123" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D123" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E123" s="2">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>308</v>
       </c>
@@ -3781,8 +4566,14 @@
       <c r="C124" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D124" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E124" s="2">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>310</v>
       </c>
@@ -3792,8 +4583,14 @@
       <c r="C125" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D125" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E125" s="2">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>313</v>
       </c>
@@ -3803,8 +4600,14 @@
       <c r="C126" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D126" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E126" s="2">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>315</v>
       </c>
@@ -3814,8 +4617,14 @@
       <c r="C127" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D127" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E127" s="2">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>318</v>
       </c>
@@ -3825,8 +4634,14 @@
       <c r="C128" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D128" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E128" s="2">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>321</v>
       </c>
@@ -3836,8 +4651,14 @@
       <c r="C129" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D129" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E129" s="2">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>324</v>
       </c>
@@ -3847,8 +4668,14 @@
       <c r="C130" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D130" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E130" s="2">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>327</v>
       </c>
@@ -3858,8 +4685,14 @@
       <c r="C131" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D131" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E131" s="2">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>330</v>
       </c>
@@ -3869,8 +4702,14 @@
       <c r="C132" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D132" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E132" s="2">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>332</v>
       </c>
@@ -3880,8 +4719,14 @@
       <c r="C133" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D133" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E133" s="2">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>334</v>
       </c>
@@ -3891,8 +4736,14 @@
       <c r="C134" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D134" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E134" s="2">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>337</v>
       </c>
@@ -3902,8 +4753,14 @@
       <c r="C135" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D135" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E135" s="2">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>340</v>
       </c>
@@ -3913,8 +4770,14 @@
       <c r="C136" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D136" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E136" s="2">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>344</v>
       </c>
@@ -3924,8 +4787,14 @@
       <c r="C137" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D137" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E137" s="2">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>346</v>
       </c>
@@ -3935,8 +4804,14 @@
       <c r="C138" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D138" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E138" s="2">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>348</v>
       </c>
@@ -3946,8 +4821,14 @@
       <c r="C139" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D139" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E139" s="2">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>351</v>
       </c>
@@ -3957,8 +4838,14 @@
       <c r="C140" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D140" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E140" s="2">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>353</v>
       </c>
@@ -3968,8 +4855,14 @@
       <c r="C141" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D141" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E141" s="2">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>356</v>
       </c>
@@ -3979,8 +4872,14 @@
       <c r="C142" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D142" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E142" s="2">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>358</v>
       </c>
@@ -3990,8 +4889,14 @@
       <c r="C143" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D143" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E143" s="2">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>360</v>
       </c>
@@ -4001,8 +4906,14 @@
       <c r="C144" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D144" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E144" s="2">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>363</v>
       </c>
@@ -4012,8 +4923,14 @@
       <c r="C145" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D145" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E145" s="2">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>365</v>
       </c>
@@ -4023,8 +4940,14 @@
       <c r="C146" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D146" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E146" s="2">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>367</v>
       </c>
@@ -4034,8 +4957,14 @@
       <c r="C147" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D147" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E147" s="2">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>369</v>
       </c>
@@ -4045,8 +4974,14 @@
       <c r="C148" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D148" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E148" s="2">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>371</v>
       </c>
@@ -4056,8 +4991,14 @@
       <c r="C149" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D149" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E149" s="2">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>374</v>
       </c>
@@ -4067,8 +5008,14 @@
       <c r="C150" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D150" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E150" s="2">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>376</v>
       </c>
@@ -4078,8 +5025,14 @@
       <c r="C151" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D151" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E151" s="2">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>378</v>
       </c>
@@ -4089,8 +5042,14 @@
       <c r="C152" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D152" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E152" s="2">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>380</v>
       </c>
@@ -4100,8 +5059,14 @@
       <c r="C153" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D153" s="2">
+        <v>5100</v>
+      </c>
+      <c r="E153" s="2">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>383</v>
       </c>
@@ -4111,8 +5076,14 @@
       <c r="C154" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D154" s="2">
+        <v>5300</v>
+      </c>
+      <c r="E154" s="2">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>386</v>
       </c>
@@ -4122,8 +5093,14 @@
       <c r="C155" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D155" s="2">
+        <v>5300</v>
+      </c>
+      <c r="E155" s="2">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>389</v>
       </c>
@@ -4133,8 +5110,14 @@
       <c r="C156" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D156" s="2">
+        <v>5300</v>
+      </c>
+      <c r="E156" s="2">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>392</v>
       </c>
@@ -4144,8 +5127,14 @@
       <c r="C157" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D157" s="2">
+        <v>5300</v>
+      </c>
+      <c r="E157" s="2">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>395</v>
       </c>
@@ -4155,8 +5144,14 @@
       <c r="C158" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D158" s="2">
+        <v>5200</v>
+      </c>
+      <c r="E158" s="2">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>398</v>
       </c>
@@ -4166,8 +5161,14 @@
       <c r="C159" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D159" s="2">
+        <v>5200</v>
+      </c>
+      <c r="E159" s="2">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>400</v>
       </c>
@@ -4177,8 +5178,14 @@
       <c r="C160" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D160" s="2">
+        <v>5200</v>
+      </c>
+      <c r="E160" s="2">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>403</v>
       </c>
@@ -4188,8 +5195,14 @@
       <c r="C161" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D161" s="2">
+        <v>5200</v>
+      </c>
+      <c r="E161" s="2">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>406</v>
       </c>
@@ -4199,8 +5212,14 @@
       <c r="C162" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D162" s="2">
+        <v>5200</v>
+      </c>
+      <c r="E162" s="2">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>408</v>
       </c>
@@ -4210,8 +5229,14 @@
       <c r="C163" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D163" s="2">
+        <v>5200</v>
+      </c>
+      <c r="E163" s="2">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>410</v>
       </c>
@@ -4221,8 +5246,14 @@
       <c r="C164" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D164" s="2">
+        <v>6100</v>
+      </c>
+      <c r="E164" s="2">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>413</v>
       </c>
@@ -4232,8 +5263,14 @@
       <c r="C165" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D165" s="2">
+        <v>6100</v>
+      </c>
+      <c r="E165" s="2">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>415</v>
       </c>
@@ -4243,8 +5280,14 @@
       <c r="C166" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D166" s="2">
+        <v>6100</v>
+      </c>
+      <c r="E166" s="2">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>418</v>
       </c>
@@ -4254,8 +5297,14 @@
       <c r="C167" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D167" s="2">
+        <v>6100</v>
+      </c>
+      <c r="E167" s="2">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>420</v>
       </c>
@@ -4265,8 +5314,14 @@
       <c r="C168" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D168" s="2">
+        <v>6100</v>
+      </c>
+      <c r="E168" s="2">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>422</v>
       </c>
@@ -4276,8 +5331,14 @@
       <c r="C169" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D169" s="2">
+        <v>6100</v>
+      </c>
+      <c r="E169" s="2">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>424</v>
       </c>
@@ -4287,8 +5348,14 @@
       <c r="C170" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D170" s="2">
+        <v>6100</v>
+      </c>
+      <c r="E170" s="2">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>426</v>
       </c>
@@ -4298,8 +5365,14 @@
       <c r="C171" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D171" s="2">
+        <v>9060</v>
+      </c>
+      <c r="E171" s="2">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>429</v>
       </c>
@@ -4309,8 +5382,14 @@
       <c r="C172" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D172" s="2">
+        <v>6300</v>
+      </c>
+      <c r="E172" s="2">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>432</v>
       </c>
@@ -4320,8 +5399,14 @@
       <c r="C173" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D173" s="2">
+        <v>6300</v>
+      </c>
+      <c r="E173" s="2">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>434</v>
       </c>
@@ -4331,8 +5416,14 @@
       <c r="C174" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D174" s="2">
+        <v>6200</v>
+      </c>
+      <c r="E174" s="2">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>437</v>
       </c>
@@ -4342,8 +5433,14 @@
       <c r="C175" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D175" s="2">
+        <v>6200</v>
+      </c>
+      <c r="E175" s="2">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>440</v>
       </c>
@@ -4353,8 +5450,14 @@
       <c r="C176" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D176" s="2">
+        <v>6200</v>
+      </c>
+      <c r="E176" s="2">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>442</v>
       </c>
@@ -4364,8 +5467,14 @@
       <c r="C177" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D177" s="2">
+        <v>6200</v>
+      </c>
+      <c r="E177" s="2">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>444</v>
       </c>
@@ -4375,8 +5484,14 @@
       <c r="C178" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D178" s="2">
+        <v>6200</v>
+      </c>
+      <c r="E178" s="2">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>447</v>
       </c>
@@ -4386,8 +5501,14 @@
       <c r="C179" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D179" s="2">
+        <v>6200</v>
+      </c>
+      <c r="E179" s="2">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>450</v>
       </c>
@@ -4397,8 +5518,14 @@
       <c r="C180" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D180" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E180" s="2">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>453</v>
       </c>
@@ -4408,8 +5535,14 @@
       <c r="C181" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D181" s="2">
+        <v>6300</v>
+      </c>
+      <c r="E181" s="2">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>456</v>
       </c>
@@ -4419,8 +5552,14 @@
       <c r="C182" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D182" s="2">
+        <v>6300</v>
+      </c>
+      <c r="E182" s="2">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>458</v>
       </c>
@@ -4430,8 +5569,14 @@
       <c r="C183" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D183" s="2">
+        <v>6100</v>
+      </c>
+      <c r="E183" s="2">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>461</v>
       </c>
@@ -4441,8 +5586,14 @@
       <c r="C184" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D184" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E184" s="2">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>464</v>
       </c>
@@ -4452,8 +5603,14 @@
       <c r="C185" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D185" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E185" s="2">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>466</v>
       </c>
@@ -4463,8 +5620,14 @@
       <c r="C186" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D186" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E186" s="2">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>468</v>
       </c>
@@ -4474,8 +5637,14 @@
       <c r="C187" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D187" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E187" s="2">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>470</v>
       </c>
@@ -4485,8 +5654,14 @@
       <c r="C188" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D188" s="2">
+        <v>2020</v>
+      </c>
+      <c r="E188" s="2">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>473</v>
       </c>
@@ -4496,8 +5671,14 @@
       <c r="C189" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D189" s="2">
+        <v>2020</v>
+      </c>
+      <c r="E189" s="2">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>476</v>
       </c>
@@ -4507,8 +5688,14 @@
       <c r="C190" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D190" s="2">
+        <v>7000</v>
+      </c>
+      <c r="E190" s="2">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>479</v>
       </c>
@@ -4518,8 +5705,14 @@
       <c r="C191" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D191" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E191" s="2">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>482</v>
       </c>
@@ -4529,8 +5722,14 @@
       <c r="C192" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D192" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E192" s="2">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>485</v>
       </c>
@@ -4540,8 +5739,14 @@
       <c r="C193" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D193" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E193" s="2">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>487</v>
       </c>
@@ -4551,8 +5756,14 @@
       <c r="C194" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D194" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E194" s="2">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>490</v>
       </c>
@@ -4562,8 +5773,14 @@
       <c r="C195" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D195" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E195" s="2">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>492</v>
       </c>
@@ -4573,8 +5790,14 @@
       <c r="C196" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D196" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E196" s="2">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>495</v>
       </c>
@@ -4584,8 +5807,14 @@
       <c r="C197" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D197" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E197" s="2">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>497</v>
       </c>
@@ -4595,8 +5824,14 @@
       <c r="C198" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D198" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E198" s="2">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>500</v>
       </c>
@@ -4606,8 +5841,14 @@
       <c r="C199" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D199" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E199" s="2">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>502</v>
       </c>
@@ -4617,8 +5858,14 @@
       <c r="C200" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D200" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E200" s="2">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>505</v>
       </c>
@@ -4628,8 +5875,14 @@
       <c r="C201" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D201" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E201" s="2">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>508</v>
       </c>
@@ -4639,8 +5892,14 @@
       <c r="C202" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D202" s="2">
+        <v>6100</v>
+      </c>
+      <c r="E202" s="2">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>511</v>
       </c>
@@ -4650,8 +5909,14 @@
       <c r="C203" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D203" s="2">
+        <v>6100</v>
+      </c>
+      <c r="E203" s="2">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>513</v>
       </c>
@@ -4661,8 +5926,14 @@
       <c r="C204" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D204" s="2">
+        <v>7000</v>
+      </c>
+      <c r="E204" s="2">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>516</v>
       </c>
@@ -4672,8 +5943,14 @@
       <c r="C205" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D205" s="2">
+        <v>6800</v>
+      </c>
+      <c r="E205" s="2">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>519</v>
       </c>
@@ -4683,8 +5960,14 @@
       <c r="C206" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D206" s="2">
+        <v>6800</v>
+      </c>
+      <c r="E206" s="2">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>521</v>
       </c>
@@ -4694,8 +5977,14 @@
       <c r="C207" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D207" s="2">
+        <v>6800</v>
+      </c>
+      <c r="E207" s="2">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>523</v>
       </c>
@@ -4705,8 +5994,14 @@
       <c r="C208" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D208" s="2">
+        <v>6800</v>
+      </c>
+      <c r="E208" s="2">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>526</v>
       </c>
@@ -4716,8 +6011,14 @@
       <c r="C209" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D209" s="2">
+        <v>6800</v>
+      </c>
+      <c r="E209" s="2">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>529</v>
       </c>
@@ -4727,8 +6028,14 @@
       <c r="C210" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D210" s="2">
+        <v>6800</v>
+      </c>
+      <c r="E210" s="2">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>531</v>
       </c>
@@ -4738,8 +6045,14 @@
       <c r="C211" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D211" s="2">
+        <v>6800</v>
+      </c>
+      <c r="E211" s="2">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>533</v>
       </c>
@@ -4749,8 +6062,14 @@
       <c r="C212" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D212" s="2">
+        <v>6800</v>
+      </c>
+      <c r="E212" s="2">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>535</v>
       </c>
@@ -4760,8 +6079,14 @@
       <c r="C213" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D213" s="2">
+        <v>6800</v>
+      </c>
+      <c r="E213" s="2">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>537</v>
       </c>
@@ -4771,8 +6096,14 @@
       <c r="C214" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D214" s="2">
+        <v>6800</v>
+      </c>
+      <c r="E214" s="2">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>539</v>
       </c>
@@ -4782,8 +6113,14 @@
       <c r="C215" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D215" s="2">
+        <v>5600</v>
+      </c>
+      <c r="E215" s="2">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>542</v>
       </c>
@@ -4793,8 +6130,14 @@
       <c r="C216" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D216" s="2">
+        <v>6600</v>
+      </c>
+      <c r="E216" s="2">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>545</v>
       </c>
@@ -4804,8 +6147,14 @@
       <c r="C217" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D217" s="2">
+        <v>5600</v>
+      </c>
+      <c r="E217" s="2">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>548</v>
       </c>
@@ -4815,8 +6164,14 @@
       <c r="C218" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D218" s="2">
+        <v>5600</v>
+      </c>
+      <c r="E218" s="2">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>550</v>
       </c>
@@ -4826,8 +6181,14 @@
       <c r="C219" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D219" s="2">
+        <v>5600</v>
+      </c>
+      <c r="E219" s="2">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>553</v>
       </c>
@@ -4837,8 +6198,14 @@
       <c r="C220" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D220" s="2">
+        <v>300</v>
+      </c>
+      <c r="E220" s="2">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>556</v>
       </c>
@@ -4848,8 +6215,14 @@
       <c r="C221" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D221" s="2">
+        <v>300</v>
+      </c>
+      <c r="E221" s="2">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>558</v>
       </c>
@@ -4859,8 +6232,14 @@
       <c r="C222" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D222" s="2">
+        <v>300</v>
+      </c>
+      <c r="E222" s="2">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>560</v>
       </c>
@@ -4870,8 +6249,14 @@
       <c r="C223" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D223" s="2">
+        <v>300</v>
+      </c>
+      <c r="E223" s="2">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>563</v>
       </c>
@@ -4881,8 +6266,14 @@
       <c r="C224" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D224" s="2">
+        <v>300</v>
+      </c>
+      <c r="E224" s="2">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>566</v>
       </c>
@@ -4892,8 +6283,14 @@
       <c r="C225" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D225" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E225" s="2">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>568</v>
       </c>
@@ -4903,8 +6300,14 @@
       <c r="C226" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D226" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E226" s="2">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>570</v>
       </c>
@@ -4914,8 +6317,14 @@
       <c r="C227" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D227" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E227" s="2">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>572</v>
       </c>
@@ -4925,8 +6334,14 @@
       <c r="C228" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D228" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E228" s="2">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>574</v>
       </c>
@@ -4936,8 +6351,14 @@
       <c r="C229" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D229" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E229" s="2">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>576</v>
       </c>
@@ -4947,8 +6368,14 @@
       <c r="C230" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D230" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E230" s="2">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>578</v>
       </c>
@@ -4958,8 +6385,14 @@
       <c r="C231" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D231" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E231" s="2">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>580</v>
       </c>
@@ -4969,8 +6402,14 @@
       <c r="C232" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D232" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E232" s="2">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>582</v>
       </c>
@@ -4980,8 +6419,14 @@
       <c r="C233" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D233" s="2">
+        <v>9000</v>
+      </c>
+      <c r="E233" s="2">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>584</v>
       </c>
@@ -4991,8 +6436,14 @@
       <c r="C234" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D234" s="2">
+        <v>2020</v>
+      </c>
+      <c r="E234" s="2">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>587</v>
       </c>
@@ -5002,8 +6453,14 @@
       <c r="C235" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D235" s="2">
+        <v>2020</v>
+      </c>
+      <c r="E235" s="2">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>589</v>
       </c>
@@ -5013,8 +6470,14 @@
       <c r="C236" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D236" s="2">
+        <v>2020</v>
+      </c>
+      <c r="E236" s="2">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>591</v>
       </c>
@@ -5024,8 +6487,14 @@
       <c r="C237" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D237" s="2">
+        <v>2010</v>
+      </c>
+      <c r="E237" s="2">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>594</v>
       </c>
@@ -5035,8 +6504,14 @@
       <c r="C238" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D238" s="2">
+        <v>2010</v>
+      </c>
+      <c r="E238" s="2">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>597</v>
       </c>
@@ -5046,8 +6521,14 @@
       <c r="C239" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D239" s="2">
+        <v>2010</v>
+      </c>
+      <c r="E239" s="2">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>600</v>
       </c>
@@ -5057,8 +6538,14 @@
       <c r="C240" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D240" s="2">
+        <v>2010</v>
+      </c>
+      <c r="E240" s="2">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>603</v>
       </c>
@@ -5068,8 +6555,14 @@
       <c r="C241" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D241" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E241" s="2">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>606</v>
       </c>
@@ -5079,8 +6572,14 @@
       <c r="C242" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D242" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E242" s="2">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>608</v>
       </c>
@@ -5090,8 +6589,14 @@
       <c r="C243" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D243" s="2">
+        <v>2120</v>
+      </c>
+      <c r="E243" s="2">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>611</v>
       </c>
@@ -5101,8 +6606,14 @@
       <c r="C244" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D244" s="2">
+        <v>5300</v>
+      </c>
+      <c r="E244" s="2">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>614</v>
       </c>
@@ -5112,8 +6623,14 @@
       <c r="C245" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D245" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E245" s="2">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>617</v>
       </c>
@@ -5123,8 +6640,14 @@
       <c r="C246" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D246" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E246" s="2">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>620</v>
       </c>
@@ -5134,8 +6657,14 @@
       <c r="C247" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D247" s="2">
+        <v>4100</v>
+      </c>
+      <c r="E247" s="2">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>623</v>
       </c>
@@ -5145,8 +6674,14 @@
       <c r="C248" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D248" s="2">
+        <v>4100</v>
+      </c>
+      <c r="E248" s="2">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>626</v>
       </c>
@@ -5156,8 +6691,14 @@
       <c r="C249" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D249" s="2">
+        <v>4100</v>
+      </c>
+      <c r="E249" s="2">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>629</v>
       </c>
@@ -5167,8 +6708,14 @@
       <c r="C250" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D250" s="2">
+        <v>4100</v>
+      </c>
+      <c r="E250" s="2">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>632</v>
       </c>
@@ -5178,8 +6725,14 @@
       <c r="C251" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D251" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E251" s="2">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>635</v>
       </c>
@@ -5189,8 +6742,14 @@
       <c r="C252" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D252" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E252" s="2">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>638</v>
       </c>
@@ -5200,8 +6759,14 @@
       <c r="C253" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D253" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E253" s="2">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>641</v>
       </c>
@@ -5211,8 +6776,14 @@
       <c r="C254" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D254" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E254" s="2">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>644</v>
       </c>
@@ -5222,8 +6793,14 @@
       <c r="C255" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D255" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E255" s="2">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>647</v>
       </c>
@@ -5233,8 +6810,14 @@
       <c r="C256" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D256" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E256" s="2">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>650</v>
       </c>
@@ -5244,8 +6827,14 @@
       <c r="C257" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D257" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E257" s="2">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>653</v>
       </c>
@@ -5255,8 +6844,14 @@
       <c r="C258" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D258" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E258" s="2">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>656</v>
       </c>
@@ -5266,8 +6861,14 @@
       <c r="C259" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D259" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E259" s="2">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>659</v>
       </c>
@@ -5277,8 +6878,14 @@
       <c r="C260" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D260" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E260" s="2">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>662</v>
       </c>
@@ -5288,8 +6895,14 @@
       <c r="C261" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D261" s="2">
+        <v>2300</v>
+      </c>
+      <c r="E261" s="2">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>665</v>
       </c>
@@ -5299,8 +6912,14 @@
       <c r="C262" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D262" s="2">
+        <v>6800</v>
+      </c>
+      <c r="E262" s="2">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>668</v>
       </c>
@@ -5309,6 +6928,12 @@
       </c>
       <c r="C263" t="s">
         <v>670</v>
+      </c>
+      <c r="D263" s="2">
+        <v>3700</v>
+      </c>
+      <c r="E263" s="2">
+        <v>1720</v>
       </c>
     </row>
   </sheetData>

</xml_diff>